<commit_message>
Added loop that retrieves gps coordinates and adds it in the excel file
</commit_message>
<xml_diff>
--- a/addresses_template.xlsx
+++ b/addresses_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao\Projects\get_coordinates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D0A71E-A878-49CE-94CF-66D525D46514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3EBC03-DFF1-48F6-9E88-A41A47FE57DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,5 +467,6 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>